<commit_message>
obtem novos dados para 2019
</commit_message>
<xml_diff>
--- a/dados/Sankey Receitas por Fonte (com DRU) - RGPS.xlsx
+++ b/dados/Sankey Receitas por Fonte (com DRU) - RGPS.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>Sankey Receitas por Fonte (com DRU) - RGPS</t>
   </si>
@@ -34,7 +34,10 @@
     <t>Métrica: Saldo R$ (Item Informação)</t>
   </si>
   <si>
-    <t xml:space="preserve">NRE3 Espécie Receita</t>
+    <t xml:space="preserve">NRE3 Espécie Receita Código Espécie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRE3 Espécie Receita Nome</t>
   </si>
   <si>
     <t xml:space="preserve">Natureza Receita Código Completo</t>
@@ -52,7 +55,10 @@
     <t xml:space="preserve">Saldo R$ (Item Informação)</t>
   </si>
   <si>
-    <t xml:space="preserve">Contribuições e outras receitas do RGPS</t>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTRIBUICOES SOCIAIS</t>
   </si>
   <si>
     <t xml:space="preserve">12140001</t>
@@ -109,6 +115,9 @@
     <t xml:space="preserve">DEMAIS CONTRIBUICOES SOCIAIS-DIV.AT.-MUL.JUR.</t>
   </si>
   <si>
+    <t xml:space="preserve">EXPLORACAO PATRIMONIO IMOBILIARIO DO ESTADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">13100111</t>
   </si>
   <si>
@@ -121,6 +130,12 @@
     <t xml:space="preserve">RECURSOS NAO-FINANCEIROS DIRETAM. ARRECADADOS</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALORES MOBILIARIOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">13210011</t>
   </si>
   <si>
@@ -145,6 +160,9 @@
     <t xml:space="preserve">DIVIDENDOS-PRINCIPAL</t>
   </si>
   <si>
+    <t xml:space="preserve">MULTAS ADMINISTRAT., CONTRATUAIS E JUDICIAIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">19100111</t>
   </si>
   <si>
@@ -163,6 +181,9 @@
     <t xml:space="preserve">MUL.P/DESCUMP.OBRIG.PREVID.ACESSORIA-PRINC.</t>
   </si>
   <si>
+    <t xml:space="preserve">INDENIZACOES, RESTITUICOES E RESSARCIMENTOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">19210111</t>
   </si>
   <si>
@@ -199,12 +220,21 @@
     <t xml:space="preserve">RESSARCIMENTO AO RGPS-PRINCIPAL</t>
   </si>
   <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMAIS RECEITAS CORRENTES</t>
+  </si>
+  <si>
     <t xml:space="preserve">19909914</t>
   </si>
   <si>
     <t xml:space="preserve">OUTRAS RECEITAS-PRIMARIAS-DIV.ATIVA-MUL.JUR.</t>
   </si>
   <si>
+    <t xml:space="preserve">ALIENACAO DE BENS IMOVEIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">22200011</t>
   </si>
   <si>
@@ -215,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">ALIENACAO DE BENS IMOVEIS-MULTAS E JUROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMAIS RECEITAS CORRENTES-INTRA</t>
   </si>
   <si>
     <t xml:space="preserve">79900211</t>
@@ -278,7 +311,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -313,6 +346,7 @@
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
+      <c r="G7"/>
     </row>
     <row r="8" ht="10.5" customHeight="1">
       <c r="A8" t="s">
@@ -323,6 +357,7 @@
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
+      <c r="G8"/>
     </row>
     <row r="9" ht="10.5" customHeight="1">
       <c r="A9" t="s">
@@ -333,6 +368,7 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
+      <c r="G9"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -353,512 +389,590 @@
       <c r="F11" t="s">
         <v>12</v>
       </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="1">
         <v>398470922973</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="1">
         <v>1457945728</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="1">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1">
         <v>6795212329</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="1">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="1">
         <v>461261819</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="1">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1">
         <v>215384461</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="1">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1">
         <v>9515027</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
         <v>21956224</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="1">
         <v>7357920</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="1">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1">
         <v>8058912</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="1">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="1">
         <v>1217519157</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="1">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="1">
         <v>332517639</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="1">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="1">
         <v>27290495</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="1">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1">
         <v>24348490</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="1">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="1">
         <v>42953</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="1">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1">
         <v>120516126</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="1">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="1">
         <v>2796</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="1">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="1">
         <v>1023794160</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="1">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="1">
         <v>1106549206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="1">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="1">
         <v>21162371</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="1">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="1">
         <v>7233450</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="1">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="1">
         <v>17862353</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="1">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1">
         <v>5812543</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="1">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="1">
         <v>35976530</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="1">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="1">
         <v>202046</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="1">
+        <v>81</v>
+      </c>
+      <c r="F36" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="1">
         <v>9973858451</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>